<commit_message>
update user management, template spp, collection,
</commit_message>
<xml_diff>
--- a/Notulen.xlsx
+++ b/Notulen.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="95">
   <si>
     <t>MARKETING</t>
   </si>
@@ -197,9 +197,6 @@
     <t>nilai rencana bayar di cetak spp belum masuk</t>
   </si>
   <si>
-    <t>kalau tanda jadi di cetak dimana?</t>
-  </si>
-  <si>
     <t>Pada text area alamat kasih keterangan 100 karakter</t>
   </si>
   <si>
@@ -269,12 +266,6 @@
     <t>penguncian saat distribusi spp belum ke reload</t>
   </si>
   <si>
-    <t>pada report daftar kwitnsi field penerimaan menjadi angsuran, nilai DPP, PPN</t>
-  </si>
-  <si>
-    <t>sorting report daftar kwitansi hanya periode saja</t>
-  </si>
-  <si>
     <t>pembuatan menu upload penerimaan VA dari bank (UTILITAS)</t>
   </si>
   <si>
@@ -290,9 +281,6 @@
     <t>tampilan di download di detail angsuran, denda, lain-lain, total</t>
   </si>
   <si>
-    <t>tgl_spk, status spk yang dapat di edit di pengaturan spk</t>
-  </si>
-  <si>
     <t>di download tagihan buat popup untuk nambah tagihan dari kwitansi lain-lain + catatan</t>
   </si>
   <si>
@@ -312,6 +300,9 @@
   </si>
   <si>
     <t>upload stok via excel ditambah field virtual account (di tabel stok belum ada, buat dengan varchar 10)</t>
+  </si>
+  <si>
+    <t>buat menu gnerate VA</t>
   </si>
 </sst>
 </file>
@@ -327,24 +318,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -359,7 +338,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -382,14 +361,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -697,8 +668,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M50"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F55" sqref="F55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -712,11 +683,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="J1" s="13" t="s">
+      <c r="J1" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -732,7 +703,7 @@
         <v>51</v>
       </c>
       <c r="M2" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -787,18 +758,18 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="10">
+    <row r="7" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
         <v>5</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="J7" s="11"/>
-      <c r="K7" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="L7" s="12"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -883,11 +854,11 @@
       <c r="C14" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="J14" s="6" t="s">
-        <v>54</v>
-      </c>
+      <c r="J14" s="6"/>
       <c r="K14" s="7"/>
-      <c r="L14" s="7"/>
+      <c r="L14" s="7" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="15" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
@@ -993,18 +964,18 @@
         <v>54</v>
       </c>
     </row>
-    <row r="23" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="10">
+    <row r="23" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="4">
         <v>9</v>
       </c>
-      <c r="B23" s="10" t="s">
+      <c r="B23" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="J23" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="K23" s="12"/>
-      <c r="L23" s="12"/>
+      <c r="J23" s="6"/>
+      <c r="K23" s="7"/>
+      <c r="L23" s="7" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24">
@@ -1200,9 +1171,6 @@
       <c r="L40" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="M40" t="s">
-        <v>59</v>
-      </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41">
@@ -1264,12 +1232,12 @@
         <v>41</v>
       </c>
       <c r="J46" s="1"/>
-      <c r="K46" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="L46" s="3"/>
+      <c r="K46" s="3"/>
+      <c r="L46" s="3" t="s">
+        <v>54</v>
+      </c>
       <c r="M46" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
@@ -1324,7 +1292,7 @@
   <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1335,11 +1303,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="K1" s="13" t="s">
+      <c r="K1" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -1352,10 +1320,10 @@
         <v>52</v>
       </c>
       <c r="M2" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="N2" s="3" t="s">
         <v>63</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -1375,7 +1343,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K4" s="3"/>
       <c r="M4" s="3" t="s">
@@ -1462,12 +1430,12 @@
         <v>6</v>
       </c>
       <c r="K11" s="3"/>
-      <c r="L11" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="M11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3" t="s">
+        <v>54</v>
+      </c>
       <c r="N11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1482,7 +1450,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -1494,11 +1462,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="K1" s="13" t="s">
+      <c r="K1" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="K2" s="3" t="s">
@@ -1508,10 +1476,10 @@
         <v>52</v>
       </c>
       <c r="M2" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="N2" s="3" t="s">
         <v>63</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -1519,7 +1487,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K3" s="3"/>
       <c r="M3" s="3" t="s">
@@ -1531,7 +1499,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="M4" s="3" t="s">
         <v>54</v>
@@ -1542,7 +1510,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="M5" s="3" t="s">
         <v>54</v>
@@ -1553,7 +1521,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M6" s="3" t="s">
         <v>54</v>
@@ -1570,10 +1538,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:N33"/>
+  <dimension ref="A2:N32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N17" sqref="N17"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1586,10 +1554,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="N2" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -1597,10 +1565,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="N3" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -1608,10 +1576,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="N4" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -1619,10 +1587,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="N5" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -1630,10 +1598,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N6" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
@@ -1641,7 +1609,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>73</v>
+        <v>72</v>
+      </c>
+      <c r="N7" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -1649,10 +1620,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="N8" t="s">
-        <v>54</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -1660,10 +1631,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="N9" t="s">
-        <v>54</v>
+        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -1671,10 +1642,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="N10" t="s">
-        <v>54</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
@@ -1682,7 +1653,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>78</v>
+        <v>77</v>
+      </c>
+      <c r="N11" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -1690,7 +1664,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>86</v>
+        <v>83</v>
+      </c>
+      <c r="N12" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
@@ -1698,7 +1675,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>77</v>
+        <v>76</v>
+      </c>
+      <c r="N13" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -1706,10 +1686,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="N14" t="s">
-        <v>54</v>
+        <v>90</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
@@ -1717,10 +1697,10 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="N15" t="s">
-        <v>54</v>
+        <v>90</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
@@ -1728,7 +1708,10 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>96</v>
+        <v>92</v>
+      </c>
+      <c r="N16" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
@@ -1736,7 +1719,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>81</v>
+        <v>80</v>
+      </c>
+      <c r="N17" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
@@ -1744,10 +1730,10 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="N18" t="s">
-        <v>54</v>
+        <v>90</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
@@ -1755,28 +1741,37 @@
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="9">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23">
         <v>1</v>
       </c>
-      <c r="B23" s="9" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="9">
+      <c r="B23" t="s">
+        <v>85</v>
+      </c>
+      <c r="N23" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24">
         <v>2</v>
       </c>
-      <c r="B24" s="9" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="9">
+      <c r="B24" t="s">
+        <v>86</v>
+      </c>
+      <c r="N24" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A25">
         <v>3</v>
       </c>
-      <c r="B25" s="9" t="s">
-        <v>90</v>
+      <c r="B25" t="s">
+        <v>87</v>
+      </c>
+      <c r="N25" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
@@ -1801,20 +1796,26 @@
         <v>54</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>6</v>
       </c>
-      <c r="B28" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B28" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="N28" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>7</v>
       </c>
-      <c r="B29" t="s">
-        <v>92</v>
+      <c r="B29" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="N29" s="4" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
@@ -1822,31 +1823,23 @@
         <v>8</v>
       </c>
       <c r="B30" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="10">
+        <v>84</v>
+      </c>
+      <c r="N30" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A31">
         <v>9</v>
       </c>
-      <c r="B31" s="10" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="10">
+      <c r="B31" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A32">
         <v>10</v>
-      </c>
-      <c r="B32" s="10" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>11</v>
-      </c>
-      <c r="B33" t="s">
-        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>